<commit_message>
Updating growth rate table
</commit_message>
<xml_diff>
--- a/Growth Rate Table.xlsx
+++ b/Growth Rate Table.xlsx
@@ -62,7 +62,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -264,7 +264,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -272,27 +272,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="3" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="9">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -622,20 +630,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1"/>
-    <row r="2" spans="1:5">
+    <row r="1" spans="1:14" ht="16" thickBot="1"/>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -652,7 +661,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:14">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -669,7 +678,7 @@
         <v>217.1945882352943</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:14">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -686,7 +695,7 @@
         <v>179.09019999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:14">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
@@ -703,7 +712,7 @@
         <v>171.59358974358975</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:14">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -720,7 +729,7 @@
         <v>112.55938461538459</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:14">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -737,7 +746,7 @@
         <v>213.52814814814815</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:14">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -754,7 +763,7 @@
         <v>221.41795454545448</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:14">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
@@ -771,7 +780,7 @@
         <v>162.72472727272728</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:14">
       <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
@@ -788,7 +797,7 @@
         <v>179.76726027397262</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:14">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
@@ -805,7 +814,7 @@
         <v>210.506386138614</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16" thickBot="1">
+    <row r="12" spans="1:14" ht="16" thickBot="1">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -822,8 +831,8 @@
         <v>178.32256983240231</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16" thickBot="1"/>
-    <row r="14" spans="1:5">
+    <row r="13" spans="1:14" ht="16" thickBot="1"/>
+    <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -839,8 +848,18 @@
       <c r="E14" s="3">
         <v>2011</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" s="1"/>
+      <c r="H14" s="2">
+        <v>2008</v>
+      </c>
+      <c r="I14" s="2">
+        <v>2009</v>
+      </c>
+      <c r="J14" s="3">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
@@ -857,8 +876,23 @@
         <f t="shared" si="0"/>
         <v>0.20098639107071858</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1.2897000000000001</v>
+      </c>
+      <c r="I15" s="10">
+        <v>1.1625000000000001</v>
+      </c>
+      <c r="J15" s="12">
+        <v>1.2010000000000001</v>
+      </c>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="4" t="s">
         <v>1</v>
       </c>
@@ -875,8 +909,23 @@
         <f t="shared" si="1"/>
         <v>0.22416790430324673</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="H16" s="10">
+        <v>1.3089</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1.2166999999999999</v>
+      </c>
+      <c r="J16" s="12">
+        <v>1.2242</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="11"/>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" s="4" t="s">
         <v>2</v>
       </c>
@@ -893,8 +942,23 @@
         <f t="shared" si="1"/>
         <v>0.14746340313350625</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" s="4">
+        <v>2</v>
+      </c>
+      <c r="H17" s="10">
+        <v>1.2103999999999999</v>
+      </c>
+      <c r="I17" s="10">
+        <v>1.1516</v>
+      </c>
+      <c r="J17" s="12">
+        <v>1.1475</v>
+      </c>
+      <c r="L17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="N17" s="11"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="4" t="s">
         <v>3</v>
       </c>
@@ -911,8 +975,23 @@
         <f t="shared" si="1"/>
         <v>-6.261428558834703E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" s="4">
+        <v>3</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.97650000000000003</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.92230000000000001</v>
+      </c>
+      <c r="J18" s="12">
+        <v>0.93740000000000001</v>
+      </c>
+      <c r="L18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="N18" s="11"/>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -929,8 +1008,23 @@
         <f t="shared" si="1"/>
         <v>0.10647371237705072</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" s="4">
+        <v>4</v>
+      </c>
+      <c r="H19" s="10">
+        <v>1.2296</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1.1409</v>
+      </c>
+      <c r="J19" s="12">
+        <v>1.1065</v>
+      </c>
+      <c r="L19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="N19" s="11"/>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
@@ -947,8 +1041,23 @@
         <f t="shared" si="1"/>
         <v>9.9238072211476291E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" s="4">
+        <v>5</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1.1541999999999999</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1.1032</v>
+      </c>
+      <c r="J20" s="12">
+        <v>1.0992</v>
+      </c>
+      <c r="L20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="N20" s="11"/>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" s="4" t="s">
         <v>6</v>
       </c>
@@ -965,8 +1074,23 @@
         <f t="shared" si="1"/>
         <v>9.8488397936673966E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" s="4">
+        <v>6</v>
+      </c>
+      <c r="H21" s="10">
+        <v>1.0625</v>
+      </c>
+      <c r="I21" s="10">
+        <v>1.0578000000000001</v>
+      </c>
+      <c r="J21" s="12">
+        <v>1.0985</v>
+      </c>
+      <c r="L21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="N21" s="11"/>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
@@ -983,8 +1107,23 @@
         <f t="shared" si="1"/>
         <v>6.7034659545604391E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" s="4">
+        <v>7</v>
+      </c>
+      <c r="H22" s="10">
+        <v>1.1379999999999999</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1.1409</v>
+      </c>
+      <c r="J22" s="12">
+        <v>1.0669999999999999</v>
+      </c>
+      <c r="L22" s="11"/>
+      <c r="M22" s="11"/>
+      <c r="N22" s="11"/>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" s="4" t="s">
         <v>8</v>
       </c>
@@ -1001,8 +1140,23 @@
         <f t="shared" si="1"/>
         <v>0.1281281467096993</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="16" thickBot="1">
+      <c r="G23" s="4">
+        <v>8</v>
+      </c>
+      <c r="H23" s="10">
+        <v>1.2650999999999999</v>
+      </c>
+      <c r="I23" s="10">
+        <v>1.1666000000000001</v>
+      </c>
+      <c r="J23" s="12">
+        <v>1.1281000000000001</v>
+      </c>
+      <c r="L23" s="11"/>
+      <c r="M23" s="11"/>
+      <c r="N23" s="11"/>
+    </row>
+    <row r="24" spans="1:14" ht="16" thickBot="1">
       <c r="A24" s="5" t="s">
         <v>9</v>
       </c>
@@ -1019,6 +1173,21 @@
         <f t="shared" si="1"/>
         <v>0.14821551535718624</v>
       </c>
+      <c r="G24" s="5">
+        <v>9</v>
+      </c>
+      <c r="H24" s="13">
+        <v>1.1755</v>
+      </c>
+      <c r="I24" s="13">
+        <v>1.1101000000000001</v>
+      </c>
+      <c r="J24" s="14">
+        <v>1.1482000000000001</v>
+      </c>
+      <c r="L24" s="11"/>
+      <c r="M24" s="11"/>
+      <c r="N24" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>